<commit_message>
Update pizza place sales dashboard.xlsx
</commit_message>
<xml_diff>
--- a/pizza place sales dashboard.xlsx
+++ b/pizza place sales dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c54a924b2259718/Documents/GitHub/proj-sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:40009_{022BF68F-FDDD-45C2-A199-6F31013BF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7106C79-C69A-4DC6-B387-E8B553B662F6}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:40009_{022BF68F-FDDD-45C2-A199-6F31013BF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24FAE36C-0850-46C1-B0B5-EF75EED538E5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="data_1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="data_2" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="pizza_place_dashboard" sheetId="3" r:id="rId3"/>
-    <sheet name="data_3" sheetId="4" r:id="rId4"/>
+    <sheet name="data_3" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">data_3!$A$1:$F$385</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5477,6 +5477,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>

</xml_diff>